<commit_message>
añadí calculo de n de cada subsubmuestra
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\R\mag-etnoc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FILES\Desktop\mag-etnoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8A9D01-6548-463C-95B7-42657948D25D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9D23B38-A94D-48EF-8F9D-1A49FFA58A7D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="660" windowWidth="19440" windowHeight="15000" xr2:uid="{463F8655-D378-4B5A-B34C-E9A4D34372C6}"/>
+    <workbookView xWindow="28680" yWindow="570" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{463F8655-D378-4B5A-B34C-E9A4D34372C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="137">
   <si>
     <t>5p</t>
   </si>
@@ -486,11 +487,17 @@
   <si>
     <t>n</t>
   </si>
+  <si>
+    <t>estudio</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="179" formatCode="0.00000000000000000"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -549,10 +556,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -867,10 +875,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE30E396-B558-44B7-ACC1-82703EC908A7}">
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,16 +890,17 @@
     <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8" customWidth="1"/>
+    <col min="10" max="10" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>135</v>
       </c>
@@ -908,7 +917,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -929,7 +938,7 @@
         <v>15.06</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -950,12 +959,12 @@
         <v>14.39</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -963,7 +972,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -974,7 +983,7 @@
         <v>0.90200000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -985,12 +994,12 @@
         <v>0.92700000000000005</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1013,7 +1022,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1038,8 +1047,9 @@
       <c r="H13">
         <v>35979</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -1065,7 +1075,7 @@
         <v>41774</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>29</v>
       </c>
@@ -1704,4 +1714,184 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BEFA05A-83CF-49C9-943F-08C50AC4C043}">
+  <dimension ref="A1:AF19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>233</v>
+      </c>
+      <c r="T10">
+        <v>235</v>
+      </c>
+      <c r="X10">
+        <v>280</v>
+      </c>
+      <c r="AB10">
+        <v>293</v>
+      </c>
+      <c r="AF10">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>136</v>
+      </c>
+      <c r="B12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>254</v>
+      </c>
+      <c r="T13">
+        <v>251</v>
+      </c>
+      <c r="X13">
+        <v>254</v>
+      </c>
+      <c r="AB13">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>